<commit_message>
Trained 2 more scan-based contrastive models, updated performance data
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amose\Documents\GitHub\CTLiverSegmentation\SPIE_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmo276\Documents\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728EFE23-6572-430E-A7A8-EE9ABE1F0E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC583881-358E-49A5-AF4E-4D55BF41FA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Tests" sheetId="9" r:id="rId1"/>
@@ -21,18 +21,30 @@
     <sheet name="Progressive Pre-Training" sheetId="5" r:id="rId6"/>
     <sheet name="Joint Training" sheetId="1" r:id="rId7"/>
     <sheet name="Contrastive Pre-Trained" sheetId="10" r:id="rId8"/>
+    <sheet name="Scan-Based Contrastive" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
   <si>
     <t>Iteration</t>
   </si>
@@ -101,6 +113,9 @@
   </si>
   <si>
     <t>Hausdorff</t>
+  </si>
+  <si>
+    <t>Scan-Based Contrastive vs Standard</t>
   </si>
 </sst>
 </file>
@@ -198,10 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -597,16 +612,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145F49CB-B145-40E7-8FE4-38A3938E89FA}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -614,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -630,7 +645,7 @@
         <v>1.2510259496342979E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -646,7 +661,7 @@
         <v>3.9205137650218612E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -654,7 +669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -670,7 +685,7 @@
         <v>0.18141858150684043</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -686,12 +701,15 @@
         <v>0.6315852060160605</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -699,8 +717,15 @@
         <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Standard Pre-Training'!B2:B11, 2, 1)</f>
         <v>0.93206183606003201</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Scan-Based Contrastive'!B2:B11, 2, 3)</f>
+        <v>0.126372672384688</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -708,13 +733,20 @@
         <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Standard Pre-Training'!C2:C11, 2, 1)</f>
         <v>0.9854985916873148</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Scan-Based Contrastive'!C2:C11, 2, 3)</f>
+        <v>5.478842049624267E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -723,7 +755,7 @@
         <v>0.85619522263495229</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -732,12 +764,12 @@
         <v>2.9371611984156704E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -746,7 +778,7 @@
         <v>0.73831284993915558</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -755,7 +787,7 @@
         <v>0.39625705698771296</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -764,7 +796,7 @@
         <v>0.73789228846612565</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -773,12 +805,12 @@
         <v>8.3169199108705419E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -787,7 +819,7 @@
         <v>1.8361830828737818E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -796,7 +828,7 @@
         <v>6.0426543279582655E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -805,7 +837,7 @@
         <v>3.3099555627477564E-12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -814,12 +846,12 @@
         <v>2.9079273386444404E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -828,7 +860,7 @@
         <v>1.6236105699244489E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -837,7 +869,7 @@
         <v>0.10091238524975189</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -846,7 +878,7 @@
         <v>6.1288711675184551E-10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -869,12 +901,12 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+    <col min="1" max="3" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -896,7 +928,7 @@
         <v>15.8362</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -907,7 +939,7 @@
         <v>20.207100000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -918,7 +950,7 @@
         <v>13.5512</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -929,7 +961,7 @@
         <v>12.761100000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -940,7 +972,7 @@
         <v>15.4732</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -951,7 +983,7 @@
         <v>18.6403</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -962,7 +994,7 @@
         <v>15.3317</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -973,7 +1005,7 @@
         <v>15.512</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -984,7 +1016,7 @@
         <v>14.584199999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -995,7 +1027,7 @@
         <v>15.769600000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +1040,7 @@
         <v>15.766659999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1037,14 +1069,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1066,7 +1098,7 @@
         <v>0.42370000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1077,7 +1109,7 @@
         <v>0.41749999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1088,7 +1120,7 @@
         <v>0.4027</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1099,7 +1131,7 @@
         <v>0.22009999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1110,7 +1142,7 @@
         <v>0.151</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1121,7 +1153,7 @@
         <v>0.32340000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1132,7 +1164,7 @@
         <v>0.374</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1143,7 +1175,7 @@
         <v>0.4103</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1154,7 +1186,7 @@
         <v>0.42749999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1165,7 +1197,7 @@
         <v>0.30159999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1210,7 @@
         <v>0.34517999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1207,12 +1239,12 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+    <col min="1" max="3" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1234,7 +1266,7 @@
         <v>0.38090000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1245,7 +1277,7 @@
         <v>0.50919999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1256,7 +1288,7 @@
         <v>0.50380000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1267,7 +1299,7 @@
         <v>0.49719999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1278,7 +1310,7 @@
         <v>0.47889999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1289,7 +1321,7 @@
         <v>0.53469999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1300,7 +1332,7 @@
         <v>0.52239999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1311,7 +1343,7 @@
         <v>0.50580000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1322,7 +1354,7 @@
         <v>0.45660000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1333,7 +1365,7 @@
         <v>0.49959999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1346,7 +1378,7 @@
         <v>0.4889099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1375,12 +1407,12 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="5" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1414,7 +1446,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1431,7 +1463,7 @@
         <v>0.49080000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1448,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1465,7 +1497,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1482,7 +1514,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1499,7 +1531,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1516,7 +1548,7 @@
         <v>0.18160000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1533,7 +1565,7 @@
         <v>0.52080000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1550,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1567,7 +1599,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1588,7 +1620,7 @@
         <v>0.38001999999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1625,12 +1657,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="5" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1647,7 +1679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1664,7 +1696,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1681,7 +1713,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1698,7 +1730,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1715,7 +1747,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1732,7 +1764,7 @@
         <v>0.52449999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1749,7 +1781,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1766,7 +1798,7 @@
         <v>0.52410000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1783,7 +1815,7 @@
         <v>0.52249999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1800,7 +1832,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1817,7 +1849,7 @@
         <v>0.50249999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1838,7 +1870,7 @@
         <v>0.5202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1875,12 +1907,12 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1897,7 +1929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1914,7 +1946,7 @@
         <v>0.49490000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1931,7 +1963,7 @@
         <v>0.49740000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1948,7 +1980,7 @@
         <v>0.49099999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1965,7 +1997,7 @@
         <v>0.48080000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1982,7 +2014,7 @@
         <v>0.45129999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1999,7 +2031,7 @@
         <v>0.4834</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2016,7 +2048,7 @@
         <v>0.49640000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2033,7 +2065,7 @@
         <v>0.47849999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2050,7 +2082,7 @@
         <v>0.44800000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2067,7 +2099,7 @@
         <v>0.49669999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2088,7 +2120,7 @@
         <v>0.48183999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2122,18 +2154,185 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DBECAB-5B38-4691-9341-2984E46A5BC3}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.90149999999999997</v>
+      </c>
+      <c r="C2" s="4">
+        <v>13.6275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="C3" s="6">
+        <v>10.0221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.90949999999999998</v>
+      </c>
+      <c r="C4" s="4">
+        <v>11.6205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="C5" s="6">
+        <v>16.0549</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.91120000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12.0365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.9274</v>
+      </c>
+      <c r="C7" s="6">
+        <v>9.3767999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.90490000000000004</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8.7723999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.90939999999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>12.695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.91279999999999994</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.9344999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.89939999999999998</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10.547000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.9073500000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
+        <v>11.468720000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6">
+        <f>_xlfn.STDEV.S(B2:B11)</f>
+        <v>8.9840908771499414E-3</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
+        <v>2.2232341566085916</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34D92F3-DA9B-4EB2-80D8-46C073400D29}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2144,140 +2343,136 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>0.90149999999999997</v>
+        <v>0.9022</v>
       </c>
       <c r="C2" s="4">
-        <v>13.6275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8.1250999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <v>0.89570000000000005</v>
+        <v>0.89980000000000004</v>
       </c>
       <c r="C3" s="6">
-        <v>10.0221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.0106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>0.90949999999999998</v>
+        <v>0.89239999999999997</v>
       </c>
       <c r="C4" s="4">
-        <v>11.6205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13.8286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>0.90169999999999995</v>
-      </c>
-      <c r="C5" s="6">
-        <v>16.0549</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>0.91120000000000001</v>
+        <v>0.82889999999999997</v>
       </c>
       <c r="C6" s="4">
-        <v>12.0365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13.5275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>0.9274</v>
+        <v>0.86209999999999998</v>
       </c>
       <c r="C7" s="6">
-        <v>9.3767999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14.0457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>0.90490000000000004</v>
+        <v>0.88560000000000005</v>
       </c>
       <c r="C8" s="4">
-        <v>8.7723999999999993</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.8329000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="6">
-        <v>0.90939999999999999</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="C9" s="6">
-        <v>12.695</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9.8215000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>0.91279999999999994</v>
+        <v>0.87329999999999997</v>
       </c>
       <c r="C10" s="4">
-        <v>9.9344999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12.109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="6">
-        <v>0.89939999999999998</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="C11" s="6">
-        <v>10.547000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12.489000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="4">
         <f>AVERAGE(B2:B11)</f>
-        <v>0.9073500000000001</v>
+        <v>0.87925555555555557</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
-        <v>11.468720000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11.53221111111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="6">
         <f>_xlfn.STDEV.S(B2:B11)</f>
-        <v>8.9840908771499414E-3</v>
+        <v>2.5462036010063666E-2</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
-        <v>2.2232341566085916</v>
+        <v>2.1377041928459506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began training limited data fine-tuned models
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmo276\Documents\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC583881-358E-49A5-AF4E-4D55BF41FA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2FD5E0-A0AE-4B39-8AD7-995BEB548512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
@@ -613,7 +613,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,7 +722,7 @@
       </c>
       <c r="H10">
         <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Scan-Based Contrastive'!B2:B11, 2, 3)</f>
-        <v>0.126372672384688</v>
+        <v>9.511709742137027E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -738,7 +738,7 @@
       </c>
       <c r="H11">
         <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Scan-Based Contrastive'!C2:C11, 2, 3)</f>
-        <v>5.478842049624267E-4</v>
+        <v>2.569038231566314E-4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -2155,7 +2155,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2322,7 +2322,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2380,8 +2380,12 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="6">
+        <v>0.89410000000000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>10.906000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
@@ -2455,11 +2459,11 @@
       </c>
       <c r="B12" s="4">
         <f>AVERAGE(B2:B11)</f>
-        <v>0.87925555555555557</v>
+        <v>0.88073999999999997</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
-        <v>11.53221111111111</v>
+        <v>11.46959</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2468,11 +2472,11 @@
       </c>
       <c r="B13" s="6">
         <f>_xlfn.STDEV.S(B2:B11)</f>
-        <v>2.5462036010063666E-2</v>
+        <v>2.4460498768422548E-2</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
-        <v>2.1377041928459506</v>
+        <v>2.0251518475029098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trained reduced data pre-trained models
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmo276\Documents\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2FD5E0-A0AE-4B39-8AD7-995BEB548512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D84974-A9AB-4EA8-AD35-CB77D2D32E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="7" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Tests" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Standard Pre-Training" sheetId="8" r:id="rId5"/>
     <sheet name="Progressive Pre-Training" sheetId="5" r:id="rId6"/>
     <sheet name="Joint Training" sheetId="1" r:id="rId7"/>
-    <sheet name="Contrastive Pre-Trained" sheetId="10" r:id="rId8"/>
+    <sheet name="Class-Based Contrastive" sheetId="10" r:id="rId8"/>
     <sheet name="Scan-Based Contrastive" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
   <si>
     <t>Iteration</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>Scan-Based Contrastive vs Standard</t>
+  </si>
+  <si>
+    <t>Full Training Set for fine-tuning</t>
+  </si>
+  <si>
+    <t>45% of training set for fine-tuning</t>
+  </si>
+  <si>
+    <t>Reduced Supervised Contrastive vs Standard</t>
   </si>
 </sst>
 </file>
@@ -612,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145F49CB-B145-40E7-8FE4-38A3938E89FA}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,7 +650,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="7">
-        <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Contrastive Pre-Trained'!B2:B11, 2, 3)</f>
+        <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Class-Based Contrastive'!B2:B11, 2, 3)</f>
         <v>1.2510259496342979E-3</v>
       </c>
     </row>
@@ -657,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="7">
-        <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Contrastive Pre-Trained'!C2:C11, 2, 3)</f>
+        <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Class-Based Contrastive'!C2:C11, 2, 3)</f>
         <v>3.9205137650218612E-4</v>
       </c>
     </row>
@@ -681,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="H6">
-        <f>_xlfn.T.TEST('Joint Training'!B2:B11, 'Contrastive Pre-Trained'!B2:B11, 2, 3)</f>
+        <f>_xlfn.T.TEST('Joint Training'!B2:B11, 'Class-Based Contrastive'!B2:B11, 2, 3)</f>
         <v>0.18141858150684043</v>
       </c>
     </row>
@@ -697,7 +706,7 @@
         <v>22</v>
       </c>
       <c r="H7">
-        <f>_xlfn.T.TEST('Joint Training'!C2:C11, 'Contrastive Pre-Trained'!C2:C11, 2, 3)</f>
+        <f>_xlfn.T.TEST('Joint Training'!C2:C11, 'Class-Based Contrastive'!C2:C11, 2, 3)</f>
         <v>0.6315852060160605</v>
       </c>
     </row>
@@ -745,6 +754,9 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -754,6 +766,13 @@
         <f>_xlfn.T.TEST('Standard Encoder'!B2:B11, 'Progressive Encoder'!B2:B11, 2, 1)</f>
         <v>0.85619522263495229</v>
       </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14">
+        <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Class-Based Contrastive'!F2:F11, 2, 3)</f>
+        <v>0.16459025818455977</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -762,6 +781,13 @@
       <c r="C15">
         <f>_xlfn.T.TEST('Standard Encoder'!C2:C11, 'Progressive Encoder'!C2:C11, 2, 1)</f>
         <v>2.9371611984156704E-3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Class-Based Contrastive'!G2:G11, 2, 3)</f>
+        <v>0.28946197248303779</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2152,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DBECAB-5B38-4691-9341-2984E46A5BC3}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2163,9 +2189,12 @@
     <col min="1" max="1" width="17.26953125" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" customWidth="1"/>
     <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2175,8 +2204,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2186,8 +2224,17 @@
       <c r="C2" s="4">
         <v>13.6275</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.81659999999999999</v>
+      </c>
+      <c r="G2" s="4">
+        <v>17.0245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2197,8 +2244,17 @@
       <c r="C3" s="6">
         <v>10.0221</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.85340000000000005</v>
+      </c>
+      <c r="G3" s="6">
+        <v>17.1648</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2208,8 +2264,17 @@
       <c r="C4" s="4">
         <v>11.6205</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="G4" s="4">
+        <v>15.6084</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2219,8 +2284,17 @@
       <c r="C5" s="6">
         <v>16.0549</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.8246</v>
+      </c>
+      <c r="G5" s="6">
+        <v>15.540100000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2230,8 +2304,13 @@
       <c r="C6" s="4">
         <v>12.0365</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2241,8 +2320,17 @@
       <c r="C7" s="6">
         <v>9.3767999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.83589999999999998</v>
+      </c>
+      <c r="G7" s="6">
+        <v>17.4953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2252,8 +2340,17 @@
       <c r="C8" s="4">
         <v>8.7723999999999993</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.82840000000000003</v>
+      </c>
+      <c r="G8" s="4">
+        <v>15.0158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2263,8 +2360,17 @@
       <c r="C9" s="6">
         <v>12.695</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E9" s="5">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.84860000000000002</v>
+      </c>
+      <c r="G9" s="6">
+        <v>17.284500000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2274,8 +2380,13 @@
       <c r="C10" s="4">
         <v>9.9344999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E10" s="3">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2285,8 +2396,17 @@
       <c r="C11" s="6">
         <v>10.547000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.86319999999999997</v>
+      </c>
+      <c r="G11" s="6">
+        <v>18.0246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2298,8 +2418,19 @@
         <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
         <v>11.468720000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <f>AVERAGE(F2:F11)</f>
+        <v>0.8384625</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" ref="G12" si="1">AVERAGE(G2:G11)</f>
+        <v>16.644749999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2308,8 +2439,27 @@
         <v>8.9840908771499414E-3</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
+        <f t="shared" ref="C13" si="2">_xlfn.STDEV.S(C2:C11)</f>
         <v>2.2232341566085916</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>1.5665880806024646E-2</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" ref="G13" si="3">_xlfn.STDEV.S(G2:G11)</f>
+        <v>1.0953873744023159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trained reduced data models
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmo276\Documents\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D84974-A9AB-4EA8-AD35-CB77D2D32E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D5FCBB-7166-44A6-BBF7-C9ADD588EBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="7" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Tests" sheetId="9" r:id="rId1"/>
@@ -621,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145F49CB-B145-40E7-8FE4-38A3938E89FA}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -771,7 +771,7 @@
       </c>
       <c r="H14">
         <f>_xlfn.T.TEST('Standard Training'!B2:B11, 'Class-Based Contrastive'!F2:F11, 2, 3)</f>
-        <v>0.16459025818455977</v>
+        <v>0.21935888052727795</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -787,7 +787,7 @@
       </c>
       <c r="H15">
         <f>_xlfn.T.TEST('Standard Training'!C2:C11, 'Class-Based Contrastive'!G2:G11, 2, 3)</f>
-        <v>0.28946197248303779</v>
+        <v>0.17754690626965675</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2180,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DBECAB-5B38-4691-9341-2984E46A5BC3}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2307,8 +2307,12 @@
       <c r="E6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="G6" s="4">
+        <v>16.856100000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
@@ -2383,8 +2387,12 @@
       <c r="E10" s="3">
         <v>9</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="4">
+        <v>0.83979999999999999</v>
+      </c>
+      <c r="G10" s="4">
+        <v>31.640699999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
@@ -2423,11 +2431,11 @@
       </c>
       <c r="F12" s="4">
         <f>AVERAGE(F2:F11)</f>
-        <v>0.8384625</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" ref="G12" si="1">AVERAGE(G2:G11)</f>
-        <v>16.644749999999998</v>
+        <v>18.165479999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2447,11 +2455,11 @@
       </c>
       <c r="F13" s="6">
         <f>_xlfn.STDEV.S(F2:F11)</f>
-        <v>1.5665880806024646E-2</v>
+        <v>1.5752036905323289E-2</v>
       </c>
       <c r="G13" s="6">
         <f t="shared" ref="G13" si="3">_xlfn.STDEV.S(G2:G11)</f>
-        <v>1.0953873744023159</v>
+        <v>4.8327137809355598</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Trained unsupervised reduced data models
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmo276\Documents\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D5FCBB-7166-44A6-BBF7-C9ADD588EBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C3A104-617D-40CB-A657-3700C5B6CBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="8" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Tests" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
   <si>
     <t>Iteration</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Reduced Supervised Contrastive vs Standard</t>
+  </si>
+  <si>
+    <t>Full Data</t>
+  </si>
+  <si>
+    <t>Reduced Data (45% of total)</t>
   </si>
 </sst>
 </file>
@@ -621,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145F49CB-B145-40E7-8FE4-38A3938E89FA}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2477,10 +2483,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34D92F3-DA9B-4EB2-80D8-46C073400D29}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2488,9 +2494,12 @@
     <col min="1" max="1" width="15.90625" customWidth="1"/>
     <col min="2" max="2" width="14.6328125" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2500,8 +2509,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2511,8 +2529,17 @@
       <c r="C2" s="4">
         <v>8.1250999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.43359999999999999</v>
+      </c>
+      <c r="G2" s="4">
+        <v>18.3917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2522,8 +2549,17 @@
       <c r="C3" s="6">
         <v>10.0106</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.43619999999999998</v>
+      </c>
+      <c r="G3" s="6">
+        <v>31.482299999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2533,8 +2569,17 @@
       <c r="C4" s="4">
         <v>13.8286</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.41639999999999999</v>
+      </c>
+      <c r="G4" s="4">
+        <v>32.652299999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2544,8 +2589,17 @@
       <c r="C5" s="6">
         <v>10.906000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.42630000000000001</v>
+      </c>
+      <c r="G5" s="6">
+        <v>32.242800000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2555,8 +2609,17 @@
       <c r="C6" s="4">
         <v>13.5275</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.8206</v>
+      </c>
+      <c r="G6" s="4">
+        <v>27.710599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2566,8 +2629,17 @@
       <c r="C7" s="6">
         <v>14.0457</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="G7" s="6">
+        <v>40.376300000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2577,8 +2649,17 @@
       <c r="C8" s="4">
         <v>9.8329000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.43419999999999997</v>
+      </c>
+      <c r="G8" s="4">
+        <v>31.841899999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2588,8 +2669,17 @@
       <c r="C9" s="6">
         <v>9.8215000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E9" s="5">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.433</v>
+      </c>
+      <c r="G9" s="6">
+        <v>25.587199999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2599,8 +2689,17 @@
       <c r="C10" s="4">
         <v>12.109</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E10" s="3">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.87270000000000003</v>
+      </c>
+      <c r="G10" s="4">
+        <v>16.2973</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2610,8 +2709,17 @@
       <c r="C11" s="6">
         <v>12.489000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.41849999999999998</v>
+      </c>
+      <c r="G11" s="6">
+        <v>22.040900000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2623,8 +2731,19 @@
         <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
         <v>11.46959</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <f>AVERAGE(F2:F11)</f>
+        <v>0.50995000000000001</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" ref="G12" si="1">AVERAGE(G2:G11)</f>
+        <v>27.862330000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2633,8 +2752,27 @@
         <v>2.4460498768422548E-2</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
+        <f t="shared" ref="C13" si="2">_xlfn.STDEV.S(C2:C11)</f>
         <v>2.0251518475029098</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>0.17811499562548527</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" ref="G13" si="3">_xlfn.STDEV.S(G2:G11)</f>
+        <v>7.3801834712288725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evaluated reduced data contrastive models
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmo276\Documents\GitHub\CTLiverSegmentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C3A104-617D-40CB-A657-3700C5B6CBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492DEF7-F449-4E59-8AFA-82662DCF3D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="8" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Tests" sheetId="9" r:id="rId1"/>
@@ -23,28 +23,17 @@
     <sheet name="Class-Based Contrastive" sheetId="10" r:id="rId8"/>
     <sheet name="Scan-Based Contrastive" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="38">
   <si>
     <t>Iteration</t>
   </si>
@@ -132,6 +121,33 @@
   <si>
     <t>Reduced Data (45% of total)</t>
   </si>
+  <si>
+    <t>1 scan</t>
+  </si>
+  <si>
+    <t>2 scans</t>
+  </si>
+  <si>
+    <t>3 scans</t>
+  </si>
+  <si>
+    <t>4 scans</t>
+  </si>
+  <si>
+    <t>5 scans</t>
+  </si>
+  <si>
+    <t>6 scans</t>
+  </si>
+  <si>
+    <t>7 scans</t>
+  </si>
+  <si>
+    <t>8 scans</t>
+  </si>
+  <si>
+    <t>9 scans</t>
+  </si>
 </sst>
 </file>
 
@@ -188,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -220,11 +236,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -233,11 +267,1013 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="71">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -250,6 +1286,891 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CPU-Net</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>('Class-Based Contrastive'!$B$24,'Class-Based Contrastive'!$B$33,'Class-Based Contrastive'!$B$42,'Class-Based Contrastive'!$B$51,'Class-Based Contrastive'!$B$65)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.22061999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21834627896645695</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30036000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54744000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84099999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3FFD-4BB5-8DB6-344E63913EF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Class-Based Contrastive'!$I$38:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.85673999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85673999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85673999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85673999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85673999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3FFD-4BB5-8DB6-344E63913EF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="489832575"/>
+        <c:axId val="611697791"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="489832575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611697791"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="611697791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489832575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E6A4566-E908-39DB-D567-516AA12F25B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3C4CFA2-164F-4739-9F43-8FD268FC5A31}" name="Table134" displayName="Table134" ref="A1:C13" totalsRowShown="0">
   <autoFilter ref="A1:C13" xr:uid="{BD452D96-A07E-4E00-990D-EAB75B65AFCF}"/>
@@ -257,6 +2178,96 @@
     <tableColumn id="1" xr3:uid="{048EEBC9-D2B1-4FDD-A2D7-4B9CD7601C94}" name="Iteration"/>
     <tableColumn id="2" xr3:uid="{63D903ED-C769-4CD7-9354-E2182A0F6E12}" name="Dice Score"/>
     <tableColumn id="3" xr3:uid="{2E45C299-4A8E-49B6-81CF-0B3AC25C6202}" name="Hausdorff Distance"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{82F705F9-F4D2-4841-83B4-18B7E815CA3F}" name="Table10" displayName="Table10" ref="A45:C50" totalsRowShown="0" headerRowDxfId="52" dataDxfId="20" headerRowBorderDxfId="54" tableBorderDxfId="55" totalsRowBorderDxfId="53">
+  <autoFilter ref="A45:C50" xr:uid="{82F705F9-F4D2-4841-83B4-18B7E815CA3F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A46:C50">
+    <sortCondition ref="A45:A50"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8C282437-5725-4450-98B8-52345604C1B8}" name="Iteration" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{FDFE7725-A109-42E9-9D36-FB6E7851F5AA}" name="Dice Score" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{FCE2B995-C997-4072-817E-1F89D4BF5E05}" name="Hausdorff Distance" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F2543028-685E-4FF6-8B35-BE5FEB147095}" name="Table11" displayName="Table11" ref="A54:C64" totalsRowShown="0" headerRowDxfId="48" dataDxfId="16" headerRowBorderDxfId="50" tableBorderDxfId="51" totalsRowBorderDxfId="49">
+  <autoFilter ref="A54:C64" xr:uid="{F2543028-685E-4FF6-8B35-BE5FEB147095}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A55:C64">
+    <sortCondition ref="A54:A64"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{807ADEC1-BDA7-41E3-8ABE-F75B7F1FF8B9}" name="Iteration" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{8AA33A74-4033-4307-9039-21C28EA58802}" name="Dice Score" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{0EB4CD20-1D14-47DC-8D82-310CBBEAE9FF}" name="Hausdorff Distance" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E9B54982-DB42-425B-A10A-57ED6EFD727B}" name="Table12" displayName="Table12" ref="A68:C73" totalsRowShown="0" headerRowDxfId="44" dataDxfId="12" headerRowBorderDxfId="46" tableBorderDxfId="47" totalsRowBorderDxfId="45">
+  <autoFilter ref="A68:C73" xr:uid="{E9B54982-DB42-425B-A10A-57ED6EFD727B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A69:C73">
+    <sortCondition ref="A68:A73"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B338A6E6-9803-43D8-BB91-85284C2EA5F0}" name="Iteration" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{79BDC265-4F0D-4265-86B8-ADA88F408442}" name="Dice Score" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{453BB242-4868-402B-8F1F-6E493000904A}" name="Hausdorff Distance" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FB3D17D9-D339-47F8-AE23-B965BE06A9D9}" name="Table14" displayName="Table14" ref="A77:C82" totalsRowShown="0" headerRowDxfId="40" dataDxfId="8" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
+  <autoFilter ref="A77:C82" xr:uid="{FB3D17D9-D339-47F8-AE23-B965BE06A9D9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A78:C82">
+    <sortCondition ref="A77:A82"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8E40B4C8-E8D8-4445-AE8F-45E6981ACCCB}" name="Iteration" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{03EF7E1D-4E84-4277-AFA3-9FAC73C3B863}" name="Dice Score" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{2E371E02-7A45-45AF-83D7-9C4DFC79AB67}" name="Hausdorff Distance" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F7368D22-A06D-4B72-B654-01A01CEAF95C}" name="Table15" displayName="Table15" ref="A86:C91" totalsRowShown="0" headerRowDxfId="36" dataDxfId="4" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
+  <autoFilter ref="A86:C91" xr:uid="{F7368D22-A06D-4B72-B654-01A01CEAF95C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A87:C91">
+    <sortCondition ref="A86:A91"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6BB25DF0-D880-4C0B-93BE-F7F9A3B6AB6D}" name="Iteration" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7C3B009D-A37F-4F73-BF8A-6E2A33601767}" name="Dice Score" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{77CA1267-1C45-431C-9D00-B4517CC1A023}" name="Hausdorff Distance" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{190D55FA-75ED-4099-A0AC-FD5E678DC527}" name="Table16" displayName="Table16" ref="A95:C100" totalsRowShown="0" headerRowDxfId="32" dataDxfId="0" headerRowBorderDxfId="34" tableBorderDxfId="35" totalsRowBorderDxfId="33">
+  <autoFilter ref="A95:C100" xr:uid="{190D55FA-75ED-4099-A0AC-FD5E678DC527}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A96:C100">
+    <sortCondition ref="A95:A100"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0BE1EE52-19DF-4EB4-A63E-05E9C7387FCE}" name="Iteration" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{EF38483A-B881-4DFC-A970-C1C616E338CF}" name="Dice Score" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{235F26A7-377E-46B0-A522-629FB35CE45E}" name="Hausdorff Distance" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -323,6 +2334,51 @@
     <tableColumn id="3" xr3:uid="{4299D94B-C521-4BAB-B01B-C6C8DF5C4B4B}" name="Hausdorff Distance"/>
     <tableColumn id="4" xr3:uid="{7B5159A6-E47A-4D2C-85A1-CCCD80A99A07}" name="Classification Accuracy"/>
     <tableColumn id="5" xr3:uid="{2E7C771C-ABF3-430E-AECC-03F696AB624A}" name="Classification F1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4854CEDD-7A8B-42C7-94DF-78377FF4822B}" name="Table7" displayName="Table7" ref="A18:C25" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="69" tableBorderDxfId="70" totalsRowBorderDxfId="68">
+  <autoFilter ref="A18:C25" xr:uid="{4854CEDD-7A8B-42C7-94DF-78377FF4822B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:C25">
+    <sortCondition descending="1" ref="B18:B25"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0605BF28-1F7C-45A0-BBBB-7F517E7A1A42}" name="Iteration" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{43609D64-12B8-4DF5-931F-CCF49D5D9098}" name="Dice Score" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{66CB39D6-3550-4519-BE05-163BBF18DE22}" name="Hausdorff Distance" dataDxfId="65"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{85F1C511-0D93-45AF-B69E-C09B42508221}" name="Table8" displayName="Table8" ref="A27:C34" totalsRowShown="0" headerRowDxfId="60" dataDxfId="28" headerRowBorderDxfId="62" tableBorderDxfId="63" totalsRowBorderDxfId="61">
+  <autoFilter ref="A27:C34" xr:uid="{85F1C511-0D93-45AF-B69E-C09B42508221}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A28:C34">
+    <sortCondition descending="1" ref="B27:B34"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B132146E-5BC4-4EF3-8699-BD5C5087D10F}" name="Iteration" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{B52C5269-D4F5-4A70-B777-1E33D04ADC40}" name="Dice Score" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{20F26483-B3FE-4F1C-8A70-7A3CD6658F5F}" name="Hausdorff Distance" dataDxfId="29"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1DD111A3-F037-43FC-8096-E2AA4552B1C9}" name="Table9" displayName="Table9" ref="A36:C41" totalsRowShown="0" headerRowDxfId="56" dataDxfId="24" headerRowBorderDxfId="58" tableBorderDxfId="59" totalsRowBorderDxfId="57">
+  <autoFilter ref="A36:C41" xr:uid="{1DD111A3-F037-43FC-8096-E2AA4552B1C9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A37:C41">
+    <sortCondition descending="1" ref="B36:B41"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3ED1779F-4F75-4C12-AD1E-CF22BE3A51A2}" name="Iteration" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0BD294F6-5AE6-4C51-AA1E-C0082EDBF068}" name="Dice Score" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{BCB271B5-CA6D-4698-84A9-5C414BA2039C}" name="Hausdorff Distance" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -631,12 +2687,12 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -644,7 +2700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -660,7 +2716,7 @@
         <v>1.2510259496342979E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -676,7 +2732,7 @@
         <v>3.9205137650218612E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -684,7 +2740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -700,7 +2756,7 @@
         <v>0.18141858150684043</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -716,7 +2772,7 @@
         <v>0.6315852060160605</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -724,7 +2780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -740,7 +2796,7 @@
         <v>9.511709742137027E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -756,7 +2812,7 @@
         <v>2.569038231566314E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -764,7 +2820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -780,7 +2836,7 @@
         <v>0.21935888052727795</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -796,12 +2852,12 @@
         <v>0.17754690626965675</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -810,7 +2866,7 @@
         <v>0.73831284993915558</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -819,7 +2875,7 @@
         <v>0.39625705698771296</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -828,7 +2884,7 @@
         <v>0.73789228846612565</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -837,12 +2893,12 @@
         <v>8.3169199108705419E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -851,7 +2907,7 @@
         <v>1.8361830828737818E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -860,7 +2916,7 @@
         <v>6.0426543279582655E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -869,7 +2925,7 @@
         <v>3.3099555627477564E-12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -878,12 +2934,12 @@
         <v>2.9079273386444404E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -892,7 +2948,7 @@
         <v>1.6236105699244489E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -901,7 +2957,7 @@
         <v>0.10091238524975189</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -910,7 +2966,7 @@
         <v>6.1288711675184551E-10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -933,12 +2989,12 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.7265625" customWidth="1"/>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +3005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -960,7 +3016,7 @@
         <v>15.8362</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -971,7 +3027,7 @@
         <v>20.207100000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -982,7 +3038,7 @@
         <v>13.5512</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -993,7 +3049,7 @@
         <v>12.761100000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1004,7 +3060,7 @@
         <v>15.4732</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1015,7 +3071,7 @@
         <v>18.6403</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1026,7 +3082,7 @@
         <v>15.3317</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1037,7 +3093,7 @@
         <v>15.512</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1048,7 +3104,7 @@
         <v>14.584199999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1059,7 +3115,7 @@
         <v>15.769600000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1072,7 +3128,7 @@
         <v>15.766659999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1101,14 +3157,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +3175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1130,7 +3186,7 @@
         <v>0.42370000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1141,7 +3197,7 @@
         <v>0.41749999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1152,7 +3208,7 @@
         <v>0.4027</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1163,7 +3219,7 @@
         <v>0.22009999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1174,7 +3230,7 @@
         <v>0.151</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1185,7 +3241,7 @@
         <v>0.32340000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1196,7 +3252,7 @@
         <v>0.374</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1207,7 +3263,7 @@
         <v>0.4103</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1218,7 +3274,7 @@
         <v>0.42749999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1229,7 +3285,7 @@
         <v>0.30159999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1242,7 +3298,7 @@
         <v>0.34517999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1271,12 +3327,12 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.7265625" customWidth="1"/>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +3343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1298,7 +3354,7 @@
         <v>0.38090000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1309,7 +3365,7 @@
         <v>0.50919999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1320,7 +3376,7 @@
         <v>0.50380000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1331,7 +3387,7 @@
         <v>0.49719999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1342,7 +3398,7 @@
         <v>0.47889999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1353,7 +3409,7 @@
         <v>0.53469999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1364,7 +3420,7 @@
         <v>0.52239999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1375,7 +3431,7 @@
         <v>0.50580000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1386,7 +3442,7 @@
         <v>0.45660000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1397,7 +3453,7 @@
         <v>0.49959999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +3466,7 @@
         <v>0.4889099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1439,12 +3495,12 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +3517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1478,7 +3534,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1495,7 +3551,7 @@
         <v>0.49080000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1512,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1529,7 +3585,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1546,7 +3602,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1563,7 +3619,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1580,7 +3636,7 @@
         <v>0.18160000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1597,7 +3653,7 @@
         <v>0.52080000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1614,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1631,7 +3687,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1652,7 +3708,7 @@
         <v>0.38001999999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1689,12 +3745,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +3767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1728,7 +3784,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1745,7 +3801,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1762,7 +3818,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1779,7 +3835,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1796,7 +3852,7 @@
         <v>0.52449999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1813,7 +3869,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1830,7 +3886,7 @@
         <v>0.52410000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1847,7 +3903,7 @@
         <v>0.52249999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1864,7 +3920,7 @@
         <v>0.52139999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1881,7 +3937,7 @@
         <v>0.50249999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1902,7 +3958,7 @@
         <v>0.5202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1939,12 +3995,12 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="20.7265625" customWidth="1"/>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +4017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1978,7 +4034,7 @@
         <v>0.49490000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1995,7 +4051,7 @@
         <v>0.49740000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2012,7 +4068,7 @@
         <v>0.49099999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2029,7 +4085,7 @@
         <v>0.48080000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2046,7 +4102,7 @@
         <v>0.45129999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2063,7 +4119,7 @@
         <v>0.4834</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2080,7 +4136,7 @@
         <v>0.49640000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2097,7 +4153,7 @@
         <v>0.47849999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2114,7 +4170,7 @@
         <v>0.44800000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2131,7 +4187,7 @@
         <v>0.49669999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2152,7 +4208,7 @@
         <v>0.48183999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2184,23 +4240,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DBECAB-5B38-4691-9341-2984E46A5BC3}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="Q53" sqref="Q53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +4276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2240,7 +4296,7 @@
         <v>17.0245</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2260,7 +4316,7 @@
         <v>17.1648</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2280,7 +4336,7 @@
         <v>15.6084</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2300,7 +4356,7 @@
         <v>15.540100000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2320,7 +4376,7 @@
         <v>16.856100000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2340,7 +4396,7 @@
         <v>17.4953</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2360,7 +4416,7 @@
         <v>15.0158</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2380,7 +4436,7 @@
         <v>17.284500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2400,7 +4456,7 @@
         <v>31.640699999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2420,7 +4476,7 @@
         <v>18.0246</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2444,7 +4500,7 @@
         <v>18.165479999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2468,7 +4524,7 @@
         <v>4.8327137809355598</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2476,8 +4532,945 @@
         <v>25</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>0</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0.253</v>
+      </c>
+      <c r="C19" s="10">
+        <v>70.4739</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0.24560000000000001</v>
+      </c>
+      <c r="C20" s="10">
+        <v>82.251199999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>2</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0.20669999999999999</v>
+      </c>
+      <c r="C21" s="10">
+        <v>76.764799999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>3</v>
+      </c>
+      <c r="B22" s="10">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="C22" s="10">
+        <v>82.526499999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>4</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0.19350000000000001</v>
+      </c>
+      <c r="C23" s="10">
+        <v>100.0067</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="10">
+        <f>AVERAGE(B16:B23)</f>
+        <v>0.22061999999999998</v>
+      </c>
+      <c r="C24" s="10">
+        <f>AVERAGE(C16:C23)</f>
+        <v>82.404619999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="11">
+        <f>_xlfn.STDEV.S(B19:B24)</f>
+        <v>2.3950231731655544E-2</v>
+      </c>
+      <c r="C25" s="11">
+        <f>_xlfn.STDEV.S(C19:C24)</f>
+        <v>9.8389152055294371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>0</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0.26850000000000002</v>
+      </c>
+      <c r="C28" s="10">
+        <v>38.649799999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>1</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0.2681</v>
+      </c>
+      <c r="C29" s="10">
+        <v>41.766399999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>2</v>
+      </c>
+      <c r="B30" s="10">
+        <v>0.26469999999999999</v>
+      </c>
+      <c r="C30" s="10">
+        <v>46.368699999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>3</v>
+      </c>
+      <c r="B31" s="10">
+        <v>0.25690000000000002</v>
+      </c>
+      <c r="C31" s="10">
+        <v>57.719799999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>4</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0.2505</v>
+      </c>
+      <c r="C32" s="10">
+        <v>32.921500000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="10">
+        <f>AVERAGE(B23:B32)</f>
+        <v>0.21834627896645695</v>
+      </c>
+      <c r="C33" s="10">
+        <f>AVERAGE(C23:C32)</f>
+        <v>51.209554400691175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="11">
+        <f>_xlfn.STDEV.S(B28:B33)</f>
+        <v>1.9046528227549139E-2</v>
+      </c>
+      <c r="C34" s="11">
+        <f>_xlfn.STDEV.S(C28:C33)</f>
+        <v>8.9284533318218777</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>0</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0.47860000000000003</v>
+      </c>
+      <c r="C37" s="10">
+        <v>16.1876</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10">
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="C38" s="10">
+        <v>35.795699999999997</v>
+      </c>
+      <c r="I38">
+        <v>0.85673999999999995</v>
+      </c>
+      <c r="J38">
+        <v>0.85673999999999995</v>
+      </c>
+      <c r="K38">
+        <v>0.85673999999999995</v>
+      </c>
+      <c r="L38">
+        <v>0.85673999999999995</v>
+      </c>
+      <c r="M38">
+        <v>0.85673999999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>2</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0.2571</v>
+      </c>
+      <c r="C39" s="10">
+        <v>29.940899999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>3</v>
+      </c>
+      <c r="B40" s="10">
+        <v>0.25669999999999998</v>
+      </c>
+      <c r="C40" s="10">
+        <v>34.3887</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>4</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0.24890000000000001</v>
+      </c>
+      <c r="C41" s="10">
+        <v>46.819699999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="10">
+        <f>AVERAGE(B37:B41)</f>
+        <v>0.30036000000000007</v>
+      </c>
+      <c r="C42" s="10">
+        <f>AVERAGE(C37:C41)</f>
+        <v>32.626519999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="11">
+        <f>_xlfn.STDEV.S(B37:B41)</f>
+        <v>9.9729724756463523E-2</v>
+      </c>
+      <c r="C43" s="11">
+        <f>_xlfn.STDEV.S(C37:C41)</f>
+        <v>11.0910547772518</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>0</v>
+      </c>
+      <c r="B46" s="10">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="C46" s="10">
+        <v>23.358699999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>1</v>
+      </c>
+      <c r="B47" s="10">
+        <v>0.44240000000000002</v>
+      </c>
+      <c r="C47" s="10">
+        <v>20.8932</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>2</v>
+      </c>
+      <c r="B48" s="10">
+        <v>0.439</v>
+      </c>
+      <c r="C48" s="10">
+        <v>21.8781</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>3</v>
+      </c>
+      <c r="B49" s="10">
+        <v>0.84009999999999996</v>
+      </c>
+      <c r="C49" s="10">
+        <v>9.9643999999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>4</v>
+      </c>
+      <c r="B50" s="10">
+        <v>0.439</v>
+      </c>
+      <c r="C50" s="10">
+        <v>25.486699999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="10">
+        <f>AVERAGE(B46:B50)</f>
+        <v>0.54744000000000004</v>
+      </c>
+      <c r="C51" s="10">
+        <f>AVERAGE(C46:C50)</f>
+        <v>20.316219999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="11">
+        <f>_xlfn.STDEV.S(B46:B50)</f>
+        <v>0.17396687328339239</v>
+      </c>
+      <c r="C52" s="11">
+        <f>_xlfn.STDEV.S(C46:C50)</f>
+        <v>6.0399317121139786</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
+        <v>0</v>
+      </c>
+      <c r="B55" s="10">
+        <v>0.81659999999999999</v>
+      </c>
+      <c r="C55" s="10">
+        <v>17.0245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>1</v>
+      </c>
+      <c r="B56" s="10">
+        <v>0.85340000000000005</v>
+      </c>
+      <c r="C56" s="10">
+        <v>17.1648</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="10">
+        <v>2</v>
+      </c>
+      <c r="B57" s="10">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="C57" s="10">
+        <v>15.6084</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="10">
+        <v>3</v>
+      </c>
+      <c r="B58" s="10">
+        <v>0.8246</v>
+      </c>
+      <c r="C58" s="10">
+        <v>15.540100000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>4</v>
+      </c>
+      <c r="B59" s="10">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="C59" s="10">
+        <v>16.856100000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="10">
+        <v>5</v>
+      </c>
+      <c r="B60" s="10">
+        <v>0.83589999999999998</v>
+      </c>
+      <c r="C60" s="10">
+        <v>17.4953</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="10">
+        <v>6</v>
+      </c>
+      <c r="B61" s="10">
+        <v>0.82840000000000003</v>
+      </c>
+      <c r="C61" s="10">
+        <v>15.0158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="10">
+        <v>7</v>
+      </c>
+      <c r="B62" s="10">
+        <v>0.84860000000000002</v>
+      </c>
+      <c r="C62" s="10">
+        <v>17.284500000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
+        <v>8</v>
+      </c>
+      <c r="B63" s="10">
+        <v>0.83979999999999999</v>
+      </c>
+      <c r="C63" s="10">
+        <v>31.640699999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="10">
+        <v>9</v>
+      </c>
+      <c r="B64" s="10">
+        <v>0.86319999999999997</v>
+      </c>
+      <c r="C64" s="10">
+        <v>18.0246</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="10">
+        <f>AVERAGE(B55:B64)</f>
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="C65" s="10">
+        <f t="shared" ref="C65" si="4">AVERAGE(C55:C64)</f>
+        <v>18.165479999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="11">
+        <f>_xlfn.STDEV.S(B55:B64)</f>
+        <v>1.5752036905323289E-2</v>
+      </c>
+      <c r="C66" s="11">
+        <f t="shared" ref="C66" si="5">_xlfn.STDEV.S(C55:C64)</f>
+        <v>4.8327137809355598</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="10">
+        <v>0</v>
+      </c>
+      <c r="B69" s="10">
+        <v>0.84489999999999998</v>
+      </c>
+      <c r="C69" s="10">
+        <v>10.6111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="10">
+        <v>1</v>
+      </c>
+      <c r="B70" s="10">
+        <v>0.78890000000000005</v>
+      </c>
+      <c r="C70" s="10">
+        <v>11.936199999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="10">
+        <v>2</v>
+      </c>
+      <c r="B71" s="10">
+        <v>0.45550000000000002</v>
+      </c>
+      <c r="C71" s="10">
+        <v>13.663399999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="10">
+        <v>3</v>
+      </c>
+      <c r="B72" s="10">
+        <v>0.72230000000000005</v>
+      </c>
+      <c r="C72" s="10">
+        <v>13.081200000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="10">
+        <v>4</v>
+      </c>
+      <c r="B73" s="10">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C73" s="10">
+        <v>17.328399999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="10">
+        <f>AVERAGE(B69:B73)</f>
+        <v>0.65205999999999997</v>
+      </c>
+      <c r="C74" s="10">
+        <f>AVERAGE(C69:C73)</f>
+        <v>13.324059999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="11">
+        <f>_xlfn.STDEV.S(B69:B73)</f>
+        <v>0.18764143465663469</v>
+      </c>
+      <c r="C75" s="11">
+        <f>_xlfn.STDEV.S(C69:C73)</f>
+        <v>2.5246375379448058</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
+        <v>0</v>
+      </c>
+      <c r="B78" s="10">
+        <v>0.86780000000000002</v>
+      </c>
+      <c r="C78" s="10">
+        <v>11.702999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="10">
+        <v>1</v>
+      </c>
+      <c r="B79" s="10">
+        <v>0.85909999999999997</v>
+      </c>
+      <c r="C79" s="10">
+        <v>9.4191000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="10">
+        <v>2</v>
+      </c>
+      <c r="B80" s="10">
+        <v>0.88380000000000003</v>
+      </c>
+      <c r="C80" s="10">
+        <v>10.1508</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="10">
+        <v>3</v>
+      </c>
+      <c r="B81" s="10">
+        <v>0.86080000000000001</v>
+      </c>
+      <c r="C81" s="10">
+        <v>15.7141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>4</v>
+      </c>
+      <c r="B82" s="10">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C82" s="10">
+        <v>12.8386</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="10">
+        <f>AVERAGE(B78:B82)</f>
+        <v>0.87209999999999999</v>
+      </c>
+      <c r="C83" s="10">
+        <f>AVERAGE(C78:C82)</f>
+        <v>11.965120000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="11">
+        <f>_xlfn.STDEV.S(B78:B82)</f>
+        <v>1.3580132547217658E-2</v>
+      </c>
+      <c r="C84" s="11">
+        <f>_xlfn.STDEV.S(C78:C82)</f>
+        <v>2.4829669826640859</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="10">
+        <v>0</v>
+      </c>
+      <c r="B87" s="10">
+        <v>0.86870000000000003</v>
+      </c>
+      <c r="C87" s="10">
+        <v>16.116399999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="10">
+        <v>1</v>
+      </c>
+      <c r="B88" s="10">
+        <v>0.45290000000000002</v>
+      </c>
+      <c r="C88" s="10">
+        <v>20.9849</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="10">
+        <v>2</v>
+      </c>
+      <c r="B89" s="10">
+        <v>0.4677</v>
+      </c>
+      <c r="C89" s="10">
+        <v>17.2774</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="10">
+        <v>3</v>
+      </c>
+      <c r="B90" s="10">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="C90" s="10">
+        <v>10.2127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="10">
+        <v>4</v>
+      </c>
+      <c r="B91" s="10">
+        <v>0.45319999999999999</v>
+      </c>
+      <c r="C91" s="10">
+        <v>16.1006</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" s="10">
+        <f>AVERAGE(B87:B91)</f>
+        <v>0.62194000000000005</v>
+      </c>
+      <c r="C92" s="10">
+        <f>AVERAGE(C87:C91)</f>
+        <v>16.138399999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="11">
+        <f>_xlfn.STDEV.S(B87:B91)</f>
+        <v>0.22465565428005579</v>
+      </c>
+      <c r="C93" s="11">
+        <f>_xlfn.STDEV.S(C87:C91)</f>
+        <v>3.8698099623883366</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="10">
+        <v>0</v>
+      </c>
+      <c r="B96" s="10">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="C96" s="10">
+        <v>12.242000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="10">
+        <v>1</v>
+      </c>
+      <c r="B97" s="10">
+        <v>0.90629999999999999</v>
+      </c>
+      <c r="C97" s="10">
+        <v>7.6818999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="10">
+        <v>2</v>
+      </c>
+      <c r="B98" s="10">
+        <v>0.90539999999999998</v>
+      </c>
+      <c r="C98" s="10">
+        <v>9.7201000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="10">
+        <v>3</v>
+      </c>
+      <c r="B99" s="10">
+        <v>0.89590000000000003</v>
+      </c>
+      <c r="C99" s="10">
+        <v>11.8787</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="10">
+        <v>4</v>
+      </c>
+      <c r="B100" s="10">
+        <v>0.90859999999999996</v>
+      </c>
+      <c r="C100" s="10">
+        <v>12.665699999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" s="10">
+        <f>AVERAGE(B96:B100)</f>
+        <v>0.90047999999999995</v>
+      </c>
+      <c r="C101" s="10">
+        <f>AVERAGE(C96:C100)</f>
+        <v>10.837680000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="11">
+        <f>_xlfn.STDEV.S(B96:B100)</f>
+        <v>9.3395396032138443E-3</v>
+      </c>
+      <c r="C102" s="11">
+        <f>_xlfn.STDEV.S(C96:C100)</f>
+        <v>2.0979410673324392</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="9">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2485,21 +5478,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34D92F3-DA9B-4EB2-80D8-46C073400D29}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2519,7 +5512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2539,7 +5532,7 @@
         <v>18.3917</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2559,7 +5552,7 @@
         <v>31.482299999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2579,7 +5572,7 @@
         <v>32.652299999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2599,7 +5592,7 @@
         <v>32.242800000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2619,7 +5612,7 @@
         <v>27.710599999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2639,7 +5632,7 @@
         <v>40.376300000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2659,7 +5652,7 @@
         <v>31.841899999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2679,7 +5672,7 @@
         <v>25.587199999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2699,7 +5692,7 @@
         <v>16.2973</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2719,7 +5712,7 @@
         <v>22.040900000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2743,7 +5736,7 @@
         <v>27.862330000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2767,7 +5760,7 @@
         <v>7.3801834712288725</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Got masks for ISBI submission
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FB860F-8EC6-4E7D-A187-1B1334AFA09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A517423D-5E3F-4779-8C24-78653566C6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="704" firstSheet="2" activeTab="8" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="T-Tests" sheetId="9" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Joint Training" sheetId="1" r:id="rId7"/>
     <sheet name="Class-Based Contrastive" sheetId="10" r:id="rId8"/>
     <sheet name="Scan-Based Contrastive" sheetId="11" r:id="rId9"/>
+    <sheet name="SimCLR" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="42">
   <si>
     <t>Iteration</t>
   </si>
@@ -153,6 +154,12 @@
   </si>
   <si>
     <t>MultiClass</t>
+  </si>
+  <si>
+    <t>vs SimCLR</t>
+  </si>
+  <si>
+    <t>Dice</t>
   </si>
 </sst>
 </file>
@@ -277,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,8 +298,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7537,12 +7542,179 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9EE4C0-4CF0-4381-B80F-8E9FC582ED4A}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.86780000000000002</v>
+      </c>
+      <c r="C2" s="4">
+        <v>12.1632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.85860000000000003</v>
+      </c>
+      <c r="C3" s="6">
+        <v>9.1182999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.85660000000000003</v>
+      </c>
+      <c r="C4" s="4">
+        <v>18.5596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.85670000000000002</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12.710800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="C6" s="4">
+        <v>11.8652</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.87039999999999995</v>
+      </c>
+      <c r="C7" s="6">
+        <v>10.9549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.86460000000000004</v>
+      </c>
+      <c r="C8" s="4">
+        <v>14.4651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.87390000000000001</v>
+      </c>
+      <c r="C9" s="6">
+        <v>14.828900000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.87029999999999996</v>
+      </c>
+      <c r="C10" s="4">
+        <v>11.159800000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.86370000000000002</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10.111700000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.86489000000000016</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
+        <v>12.59375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6">
+        <f>_xlfn.STDEV.S(B2:B11)</f>
+        <v>6.0381104476299168E-3</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
+        <v>2.7447007225034796</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE7B198-A19B-493B-B085-8D5AE4C3117E}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7975,7 +8147,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8145,7 +8317,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8313,7 +8485,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8563,7 +8735,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9063,8 +9235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DBECAB-5B38-4691-9341-2984E46A5BC3}">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9075,6 +9247,7 @@
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18.42578125" customWidth="1"/>
     <col min="11" max="11" width="24.140625" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" customWidth="1"/>
@@ -9605,6 +9778,9 @@
       <c r="E18" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
       <c r="M18">
         <f>_xlfn.T.TEST('Class-Based Contrastive'!O2:O11, 'Standard Training'!C16:C25, 2, 3)</f>
         <v>0.86228730050467084</v>
@@ -9620,6 +9796,13 @@
       <c r="C19" s="6">
         <v>84.214699999999993</v>
       </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19">
+        <f>_xlfn.T.TEST(B2:B11, SimCLR!B2:B11, 2, 3)</f>
+        <v>1.6427687072287007E-9</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -9630,6 +9813,13 @@
       </c>
       <c r="C20" s="6">
         <v>70.755099999999999</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20">
+        <f>_xlfn.T.TEST('Class-Based Contrastive'!C2:C11, SimCLR!C2:C11, 2, 3)</f>
+        <v>1.9872755606033248E-3</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -10646,8 +10836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34D92F3-DA9B-4EB2-80D8-46C073400D29}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11043,7 +11233,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -11056,8 +11251,15 @@
       <c r="E18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.T.TEST(B2:B11, SimCLR!B2:B11, 2, 3)</f>
+        <v>7.8989740317153723E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>0</v>
       </c>
@@ -11067,8 +11269,15 @@
       <c r="C19" s="6">
         <v>58.446899999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19">
+        <f>_xlfn.T.TEST(C2:C11, SimCLR!C2:C11, 2, 3)</f>
+        <v>1.2495868391070274E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -11079,7 +11288,7 @@
         <v>40.997399999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>2</v>
       </c>
@@ -11090,7 +11299,7 @@
         <v>44.982300000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>3</v>
       </c>
@@ -11101,7 +11310,7 @@
         <v>57.547899999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>4</v>
       </c>
@@ -11112,7 +11321,7 @@
         <v>37.638800000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -11125,7 +11334,7 @@
         <v>47.92266</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>6</v>
       </c>
@@ -11138,7 +11347,7 @@
         <v>9.5625257141092241</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
@@ -11152,7 +11361,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>0</v>
       </c>
@@ -11163,7 +11372,7 @@
         <v>59.244900000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -11174,7 +11383,7 @@
         <v>39.353499999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>2</v>
       </c>
@@ -11185,7 +11394,7 @@
         <v>41.850999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>3</v>
       </c>
@@ -11196,7 +11405,7 @@
         <v>53.451999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>4</v>
       </c>
@@ -11588,57 +11797,57 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="13">
+      <c r="A69" s="6">
         <v>5</v>
       </c>
-      <c r="B69" s="13">
+      <c r="B69" s="6">
         <v>0.42599999999999999</v>
       </c>
-      <c r="C69" s="13">
+      <c r="C69" s="6">
         <v>17.747399999999999</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="13">
+      <c r="A70" s="6">
         <v>6</v>
       </c>
-      <c r="B70" s="13">
+      <c r="B70" s="6">
         <v>0.44259999999999999</v>
       </c>
-      <c r="C70" s="13">
+      <c r="C70" s="6">
         <v>11.3957</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
+      <c r="A71" s="6">
         <v>7</v>
       </c>
-      <c r="B71" s="13">
+      <c r="B71" s="6">
         <v>0.43280000000000002</v>
       </c>
-      <c r="C71" s="13">
+      <c r="C71" s="6">
         <v>12.8269</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="13">
+      <c r="A72" s="6">
         <v>8</v>
       </c>
-      <c r="B72" s="13">
+      <c r="B72" s="6">
         <v>0.44529999999999997</v>
       </c>
-      <c r="C72" s="13">
+      <c r="C72" s="6">
         <v>11.0306</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="14">
+      <c r="A73" s="10">
         <v>9</v>
       </c>
-      <c r="B73" s="14">
+      <c r="B73" s="10">
         <v>0.42570000000000002</v>
       </c>
-      <c r="C73" s="14">
+      <c r="C73" s="10">
         <v>12.0182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added TotalSegmentator with fine tuning results
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTLiverSegmentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E400E0A-F2A5-4853-898B-79642C5F6BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2585A5A7-D42C-43E2-9A92-5A44141A000C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="704" firstSheet="2" activeTab="7" xr2:uid="{208B1CEA-3373-4165-BDCF-E47B75CA6FD7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="44">
   <si>
     <t>Iteration</t>
   </si>
@@ -161,6 +161,12 @@
   <si>
     <t>Dice</t>
   </si>
+  <si>
+    <t>TotalSegmentator w/ FineTuning</t>
+  </si>
+  <si>
+    <t>TotalSegmentator w/ Fine Tuning</t>
+  </si>
 </sst>
 </file>
 
@@ -284,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -298,10 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,6 +316,84 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -390,11 +471,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -472,11 +580,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -554,11 +689,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -636,11 +798,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -718,11 +907,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -800,11 +1016,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -882,11 +1125,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -964,11 +1234,38 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -993,300 +1290,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -7838,45 +7841,45 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{4F3D2566-8DB9-4AC6-A27C-60E6BD37336D}" name="Table18" displayName="Table18" ref="A15:C20" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="70" tableBorderDxfId="71" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{4F3D2566-8DB9-4AC6-A27C-60E6BD37336D}" name="Table18" displayName="Table18" ref="A15:C20" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="A15:C20" xr:uid="{4F3D2566-8DB9-4AC6-A27C-60E6BD37336D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:C20">
     <sortCondition ref="A15:A20"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{53EF963B-D662-4E98-B94B-87399714F74D}" name="Iteration" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{0A35C664-EABE-417D-B478-00567ED0F6FA}" name="Dice Score" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{A48DC984-B1EE-421D-9876-9CB5407B74E5}" name="Hausdorff Distance" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{53EF963B-D662-4E98-B94B-87399714F74D}" name="Iteration" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{0A35C664-EABE-417D-B478-00567ED0F6FA}" name="Dice Score" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{A48DC984-B1EE-421D-9876-9CB5407B74E5}" name="Hausdorff Distance" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{E8A9E7EC-FBB8-41D4-9968-0D62BE428242}" name="Table19" displayName="Table19" ref="A24:C29" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" headerRowBorderDxfId="67" tableBorderDxfId="68" totalsRowBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{E8A9E7EC-FBB8-41D4-9968-0D62BE428242}" name="Table19" displayName="Table19" ref="A24:C29" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A24:C29" xr:uid="{E8A9E7EC-FBB8-41D4-9968-0D62BE428242}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:C29">
     <sortCondition ref="A24:A29"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4B4BA720-93A1-4E5A-A04E-2D1E12FF7AC4}" name="Iteration" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{1F83F8F0-9F02-4733-9B90-333ED19D1519}" name="Dice Score" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{B49154BA-4499-4674-BC1C-3CB1A6371D28}" name="Hausdorff Distance" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{4B4BA720-93A1-4E5A-A04E-2D1E12FF7AC4}" name="Iteration" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{1F83F8F0-9F02-4733-9B90-333ED19D1519}" name="Dice Score" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{B49154BA-4499-4674-BC1C-3CB1A6371D28}" name="Hausdorff Distance" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{78488E60-6979-4C32-A6F2-7EE44157A047}" name="Table20" displayName="Table20" ref="A33:C38" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" headerRowBorderDxfId="64" tableBorderDxfId="65" totalsRowBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{78488E60-6979-4C32-A6F2-7EE44157A047}" name="Table20" displayName="Table20" ref="A33:C38" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A33:C38" xr:uid="{78488E60-6979-4C32-A6F2-7EE44157A047}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:C38">
     <sortCondition ref="A33:A38"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8A82E1BC-745A-40AA-9494-735AA9BC0565}" name="Iteration" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{85AB1E52-41E6-44C4-B019-A6B1C8482760}" name="Dice Score" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{864B0F8E-692E-49F3-9E3A-E033C9985B87}" name="Hausdorff Distance" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{8A82E1BC-745A-40AA-9494-735AA9BC0565}" name="Iteration" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{85AB1E52-41E6-44C4-B019-A6B1C8482760}" name="Dice Score" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{864B0F8E-692E-49F3-9E3A-E033C9985B87}" name="Hausdorff Distance" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7895,90 +7898,90 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F7A21220-1AD9-4A8A-BA31-59260B10384B}" name="Table21" displayName="Table21" ref="A42:C47" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowBorderDxfId="61" tableBorderDxfId="62" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F7A21220-1AD9-4A8A-BA31-59260B10384B}" name="Table21" displayName="Table21" ref="A42:C47" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="A42:C47" xr:uid="{F7A21220-1AD9-4A8A-BA31-59260B10384B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:C47">
     <sortCondition ref="A42:A47"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{73CA3CA8-39DC-4D23-837F-1CCC7D520CA1}" name="Iteration" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{937C2A8C-A668-4A06-B2CF-D8C5288222B8}" name="Dice Score" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{47A65F9C-1DA4-4999-9239-27DC98D4570C}" name="Hausdorff Distance" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{73CA3CA8-39DC-4D23-837F-1CCC7D520CA1}" name="Iteration" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{937C2A8C-A668-4A06-B2CF-D8C5288222B8}" name="Dice Score" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{47A65F9C-1DA4-4999-9239-27DC98D4570C}" name="Hausdorff Distance" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7570FEDA-2A01-496A-91B1-39AC4F139C96}" name="Table22" displayName="Table22" ref="A51:C56" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="58" tableBorderDxfId="59" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7570FEDA-2A01-496A-91B1-39AC4F139C96}" name="Table22" displayName="Table22" ref="A51:C56" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A51:C56" xr:uid="{7570FEDA-2A01-496A-91B1-39AC4F139C96}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A52:C56">
     <sortCondition ref="A51:A56"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54E78634-2B65-4CE8-9954-8B9FF8F7BEB5}" name="Iteration" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F57FCE52-D98F-4033-B6CC-8DC4B55E9A57}" name="Dice Score" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{B951249D-D146-4CE3-AEFE-BF8F46D69854}" name="Hausdorff Distance" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{54E78634-2B65-4CE8-9954-8B9FF8F7BEB5}" name="Iteration" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{F57FCE52-D98F-4033-B6CC-8DC4B55E9A57}" name="Dice Score" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B951249D-D146-4CE3-AEFE-BF8F46D69854}" name="Hausdorff Distance" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{28AD94E1-D662-46B1-8C5F-9C958A4FED86}" name="Table23" displayName="Table23" ref="A60:C65" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="55" tableBorderDxfId="56" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{28AD94E1-D662-46B1-8C5F-9C958A4FED86}" name="Table23" displayName="Table23" ref="A60:C65" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A60:C65" xr:uid="{28AD94E1-D662-46B1-8C5F-9C958A4FED86}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A61:C65">
     <sortCondition ref="A60:A65"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{795075D3-1E85-446F-92DA-563C8655E2D6}" name="Iteration" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{6CA5CB58-C528-4CD2-904B-E6276EDFF7F2}" name="Dice Score" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{E717D37C-3617-441B-80FB-11A563DAE066}" name="Hausdorff Distance" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{795075D3-1E85-446F-92DA-563C8655E2D6}" name="Iteration" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{6CA5CB58-C528-4CD2-904B-E6276EDFF7F2}" name="Dice Score" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{E717D37C-3617-441B-80FB-11A563DAE066}" name="Hausdorff Distance" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{EC3838F9-6CB8-490A-9EF3-8FCD7254CF0A}" name="Table24" displayName="Table24" ref="A69:C74" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="52" tableBorderDxfId="53" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{EC3838F9-6CB8-490A-9EF3-8FCD7254CF0A}" name="Table24" displayName="Table24" ref="A69:C74" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A69:C74" xr:uid="{EC3838F9-6CB8-490A-9EF3-8FCD7254CF0A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A70:C74">
     <sortCondition ref="A69:A74"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C2D24FD1-111A-47EA-BFED-05D9803D1EBC}" name="Iteration" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{E3479DB4-8990-4426-B76D-619E4197AE96}" name="Dice Score" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{C7977E73-E9CD-43E1-AA95-0BE2C0895A9D}" name="Hausdorff Distance" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{C2D24FD1-111A-47EA-BFED-05D9803D1EBC}" name="Iteration" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{E3479DB4-8990-4426-B76D-619E4197AE96}" name="Dice Score" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{C7977E73-E9CD-43E1-AA95-0BE2C0895A9D}" name="Hausdorff Distance" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{26889ECD-1B6E-45EE-82DC-9138DC8542BC}" name="Table34" displayName="Table34" ref="A78:C83" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="49" tableBorderDxfId="50" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{26889ECD-1B6E-45EE-82DC-9138DC8542BC}" name="Table34" displayName="Table34" ref="A78:C83" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A78:C83" xr:uid="{26889ECD-1B6E-45EE-82DC-9138DC8542BC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A79:C83">
     <sortCondition ref="A78:A83"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EDC97D37-4229-4F9D-8C5E-2ADD04F7FA9D}" name="Iteration" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{3F1937B1-CC3F-406D-9E69-1F583F40E23E}" name="Dice Score" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{5788025C-4A15-44D1-87F1-1F2F52F9B17C}" name="Hausdorff Distance" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{EDC97D37-4229-4F9D-8C5E-2ADD04F7FA9D}" name="Iteration" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{3F1937B1-CC3F-406D-9E69-1F583F40E23E}" name="Dice Score" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5788025C-4A15-44D1-87F1-1F2F52F9B17C}" name="Hausdorff Distance" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{D19F0CF6-9203-4F9B-BEF2-FB20A829B000}" name="Table35" displayName="Table35" ref="A87:C92" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="46" tableBorderDxfId="47" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{D19F0CF6-9203-4F9B-BEF2-FB20A829B000}" name="Table35" displayName="Table35" ref="A87:C92" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A87:C92" xr:uid="{D19F0CF6-9203-4F9B-BEF2-FB20A829B000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A88:C92">
     <sortCondition ref="A87:A92"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5D9B42C8-F0BA-4E81-89F0-73016538088B}" name="Iteration" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{535E3AD6-7529-4C06-B50C-818704A248C5}" name="Dice Score" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{79147823-E1CB-4C0D-81D1-115CA441A579}" name="Hausdorff Distance" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5D9B42C8-F0BA-4E81-89F0-73016538088B}" name="Iteration" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{535E3AD6-7529-4C06-B50C-818704A248C5}" name="Dice Score" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{79147823-E1CB-4C0D-81D1-115CA441A579}" name="Hausdorff Distance" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8664,10 +8667,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9EE4C0-4CF0-4381-B80F-8E9FC582ED4A}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8675,9 +8678,12 @@
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8687,8 +8693,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8698,8 +8713,17 @@
       <c r="C2" s="4">
         <v>12.1632</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.27289999999999998</v>
+      </c>
+      <c r="H2" s="4">
+        <v>38.632800000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -8709,8 +8733,17 @@
       <c r="C3" s="6">
         <v>9.1182999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.2858</v>
+      </c>
+      <c r="H3" s="6">
+        <v>43.701700000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8720,8 +8753,17 @@
       <c r="C4" s="4">
         <v>18.5596</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.26729999999999998</v>
+      </c>
+      <c r="H4" s="4">
+        <v>60.988500000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -8731,8 +8773,17 @@
       <c r="C5" s="6">
         <v>12.710800000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.51219999999999999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>28.6938</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8742,8 +8793,17 @@
       <c r="C6" s="4">
         <v>11.8652</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.74390000000000001</v>
+      </c>
+      <c r="H6" s="4">
+        <v>18.0153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -8753,8 +8813,17 @@
       <c r="C7" s="6">
         <v>10.9549</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5">
+        <v>6</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.27310000000000001</v>
+      </c>
+      <c r="H7" s="6">
+        <v>41.214100000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8764,8 +8833,17 @@
       <c r="C8" s="4">
         <v>14.4651</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <v>7</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H8" s="4">
+        <v>51.502800000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -8775,8 +8853,17 @@
       <c r="C9" s="6">
         <v>14.828900000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.2979</v>
+      </c>
+      <c r="H9" s="6">
+        <v>39.164400000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8786,8 +8873,17 @@
       <c r="C10" s="4">
         <v>11.159800000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <v>9</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.27529999999999999</v>
+      </c>
+      <c r="H10" s="4">
+        <v>46.131900000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -8797,8 +8893,17 @@
       <c r="C11" s="6">
         <v>10.111700000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.27939999999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <v>39.059199999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -8810,8 +8915,19 @@
         <f t="shared" ref="C12" si="0">AVERAGE(C2:C11)</f>
         <v>12.59375</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="4">
+        <f>AVERAGE(G2:G11)</f>
+        <v>0.34977999999999998</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" ref="H12" si="1">AVERAGE(H2:H11)</f>
+        <v>40.710449999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -8820,17 +8936,27 @@
         <v>6.0381104476299168E-3</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" ref="C13" si="1">_xlfn.STDEV.S(C2:C11)</f>
+        <f t="shared" ref="C13" si="2">_xlfn.STDEV.S(C2:C11)</f>
         <v>2.7447007225034796</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6">
+        <f>_xlfn.STDEV.S(G2:G11)</f>
+        <v>0.15676003458931878</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" ref="H13" si="3">_xlfn.STDEV.S(H2:H11)</f>
+        <v>11.714998590339954</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>0</v>
       </c>
@@ -8840,104 +8966,90 @@
       <c r="C15" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="14"/>
       <c r="E15" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>1</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="6">
         <v>0.15740000000000001</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="6">
         <v>95.767600000000002</v>
       </c>
-      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="6">
         <v>2</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="6">
         <v>0.19489999999999999</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="6">
         <v>96.348399999999998</v>
       </c>
-      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="A18" s="6">
         <v>3</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="6">
         <v>0.18279999999999999</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="6">
         <v>81.941900000000004</v>
       </c>
-      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="6">
         <v>4</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="6">
         <v>0.1615</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="6">
         <v>86.222200000000001</v>
       </c>
-      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20" s="6">
         <v>5</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="6">
         <v>0.1971</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="6">
         <v>101.2525</v>
       </c>
-      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="6">
         <f>AVERAGE(B16:B20)</f>
         <v>0.17873999999999998</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="6">
         <f>AVERAGE(C16:C20)</f>
         <v>92.306520000000006</v>
       </c>
-      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="6">
         <f>_xlfn.STDEV.S(B16:B20)</f>
         <v>1.8488726294691036E-2</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="6">
         <f>_xlfn.STDEV.S(C16:C20)</f>
         <v>7.9496969198202745</v>
       </c>
-      <c r="D22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
@@ -8949,104 +9061,90 @@
       <c r="C24" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="14"/>
       <c r="E24" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25" s="6">
         <v>1</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="6">
         <v>0.28549999999999998</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="6">
         <v>37.651499999999999</v>
       </c>
-      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="6">
         <v>2</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="6">
         <v>0.26769999999999999</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="6">
         <v>54.393900000000002</v>
       </c>
-      <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="A27" s="6">
         <v>3</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="6">
         <v>0.30599999999999999</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="6">
         <v>31.835799999999999</v>
       </c>
-      <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="6">
         <v>4</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="6">
         <v>0.29060000000000002</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="6">
         <v>64.045400000000001</v>
       </c>
-      <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="A29" s="6">
         <v>5</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="6">
         <v>0.26269999999999999</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="6">
         <v>64.946899999999999</v>
       </c>
-      <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="6">
         <f>AVERAGE(B25:B29)</f>
         <v>0.28249999999999997</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="6">
         <f>AVERAGE(C25:C29)</f>
         <v>50.5747</v>
       </c>
-      <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="6">
         <f>_xlfn.STDEV.S(B25:B29)</f>
         <v>1.7592185765276585E-2</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="6">
         <f>_xlfn.STDEV.S(C25:C29)</f>
         <v>15.172027315260131</v>
       </c>
-      <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -9058,104 +9156,90 @@
       <c r="C33" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="14"/>
       <c r="E33" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="A34" s="6">
         <v>1</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="6">
         <v>0.2676</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="6">
         <v>44.520200000000003</v>
       </c>
-      <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="A35" s="6">
         <v>2</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="6">
         <v>0.22120000000000001</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="6">
         <v>65.411600000000007</v>
       </c>
-      <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="A36" s="6">
         <v>3</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="6">
         <v>0.2276</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="6">
         <v>58.474699999999999</v>
       </c>
-      <c r="D36" s="14"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="A37" s="6">
         <v>4</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="6">
         <v>0.2414</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="6">
         <v>63.030299999999997</v>
       </c>
-      <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+      <c r="A38" s="6">
         <v>5</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="6">
         <v>0.24010000000000001</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="6">
         <v>67.628699999999995</v>
       </c>
-      <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="6">
         <f>AVERAGE(B34:B38)</f>
         <v>0.23957999999999999</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="6">
         <f>AVERAGE(C34:C38)</f>
         <v>59.813099999999999</v>
       </c>
-      <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="6">
         <f>_xlfn.STDEV.S(B34:B38)</f>
         <v>1.7818866406143798E-2</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="6">
         <f>_xlfn.STDEV.S(C34:C38)</f>
         <v>9.1983869023324161</v>
       </c>
-      <c r="D40" s="14"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
@@ -9167,104 +9251,90 @@
       <c r="C42" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="14"/>
       <c r="E42" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+      <c r="A43" s="6">
         <v>1</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="6">
         <v>0.4577</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="6">
         <v>23.7454</v>
       </c>
-      <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
+      <c r="A44" s="6">
         <v>2</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="6">
         <v>0.52359999999999995</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="6">
         <v>23.002500000000001</v>
       </c>
-      <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
+      <c r="A45" s="6">
         <v>3</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="6">
         <v>0.39219999999999999</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="6">
         <v>33.742400000000004</v>
       </c>
-      <c r="D45" s="14"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
+      <c r="A46" s="6">
         <v>4</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="6">
         <v>0.40200000000000002</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="6">
         <v>32.106000000000002</v>
       </c>
-      <c r="D46" s="14"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="15">
+      <c r="A47" s="6">
         <v>5</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="6">
         <v>0.39979999999999999</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="6">
         <v>35.446899999999999</v>
       </c>
-      <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="6">
         <f>AVERAGE(B43:B47)</f>
         <v>0.43506</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="6">
         <f>AVERAGE(C43:C47)</f>
         <v>29.608640000000001</v>
       </c>
-      <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="6">
         <f>_xlfn.STDEV.S(B43:B47)</f>
         <v>5.5957823402988209E-2</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="6">
         <f>_xlfn.STDEV.S(C43:C47)</f>
         <v>5.8186924547530294</v>
       </c>
-      <c r="D49" s="14"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
@@ -9276,104 +9346,90 @@
       <c r="C51" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="14"/>
       <c r="E51" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="15">
+      <c r="A52" s="6">
         <v>1</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="6">
         <v>0.40329999999999999</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C52" s="6">
         <v>33.8611</v>
       </c>
-      <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="15">
+      <c r="A53" s="6">
         <v>2</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="6">
         <v>0.39460000000000001</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="6">
         <v>38.575699999999998</v>
       </c>
-      <c r="D53" s="14"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="15">
+      <c r="A54" s="6">
         <v>3</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="6">
         <v>0.39689999999999998</v>
       </c>
-      <c r="C54" s="15">
+      <c r="C54" s="6">
         <v>41.032800000000002</v>
       </c>
-      <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="15">
+      <c r="A55" s="6">
         <v>4</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="6">
         <v>0.40660000000000002</v>
       </c>
-      <c r="C55" s="15">
+      <c r="C55" s="6">
         <v>36.636299999999999</v>
       </c>
-      <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="15">
+      <c r="A56" s="6">
         <v>5</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="6">
         <v>0.38950000000000001</v>
       </c>
-      <c r="C56" s="15">
+      <c r="C56" s="6">
         <v>44.318100000000001</v>
       </c>
-      <c r="D56" s="14"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="6">
         <f>AVERAGE(B52:B56)</f>
         <v>0.39818000000000003</v>
       </c>
-      <c r="C57" s="15">
+      <c r="C57" s="6">
         <f>AVERAGE(C52:C56)</f>
         <v>38.884800000000006</v>
       </c>
-      <c r="D57" s="14"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="6">
         <f>_xlfn.STDEV.S(B52:B56)</f>
         <v>6.8357150320943021E-3</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C58" s="6">
         <f>_xlfn.STDEV.S(C52:C56)</f>
         <v>4.0163263575063226</v>
       </c>
-      <c r="D58" s="14"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
@@ -9385,104 +9441,90 @@
       <c r="C60" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="14"/>
       <c r="E60" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="15">
+      <c r="A61" s="6">
         <v>1</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="6">
         <v>0.42249999999999999</v>
       </c>
-      <c r="C61" s="15">
+      <c r="C61" s="6">
         <v>32.052999999999997</v>
       </c>
-      <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="15">
+      <c r="A62" s="6">
         <v>2</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="6">
         <v>0.83320000000000005</v>
       </c>
-      <c r="C62" s="15">
+      <c r="C62" s="6">
         <v>13.066800000000001</v>
       </c>
-      <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="15">
+      <c r="A63" s="6">
         <v>3</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="6">
         <v>0.87719999999999998</v>
       </c>
-      <c r="C63" s="15">
+      <c r="C63" s="6">
         <v>11.4306</v>
       </c>
-      <c r="D63" s="14"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="15">
+      <c r="A64" s="6">
         <v>4</v>
       </c>
-      <c r="B64" s="15">
+      <c r="B64" s="6">
         <v>0.84609999999999996</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="6">
         <v>16.140899999999998</v>
       </c>
-      <c r="D64" s="14"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="15">
+      <c r="A65" s="6">
         <v>5</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B65" s="6">
         <v>0.8196</v>
       </c>
-      <c r="C65" s="15">
+      <c r="C65" s="6">
         <v>13.795</v>
       </c>
-      <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="6">
         <f>AVERAGE(B61:B65)</f>
         <v>0.75971999999999995</v>
       </c>
-      <c r="C66" s="15">
+      <c r="C66" s="6">
         <f>AVERAGE(C61:C65)</f>
         <v>17.297260000000001</v>
       </c>
-      <c r="D66" s="14"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="15">
+      <c r="B67" s="6">
         <f>_xlfn.STDEV.S(B61:B65)</f>
         <v>0.18971380287158857</v>
       </c>
-      <c r="C67" s="15">
+      <c r="C67" s="6">
         <f>_xlfn.STDEV.S(C61:C65)</f>
         <v>8.4209463225934336</v>
       </c>
-      <c r="D67" s="14"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
@@ -9494,104 +9536,90 @@
       <c r="C69" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D69" s="14"/>
       <c r="E69" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="15">
+      <c r="A70" s="6">
         <v>1</v>
       </c>
-      <c r="B70" s="15">
+      <c r="B70" s="6">
         <v>0.85150000000000003</v>
       </c>
-      <c r="C70" s="15">
+      <c r="C70" s="6">
         <v>8.4338999999999995</v>
       </c>
-      <c r="D70" s="14"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="15">
+      <c r="A71" s="6">
         <v>2</v>
       </c>
-      <c r="B71" s="15">
+      <c r="B71" s="6">
         <v>0.86129999999999995</v>
       </c>
-      <c r="C71" s="15">
+      <c r="C71" s="6">
         <v>9.5946999999999996</v>
       </c>
-      <c r="D71" s="14"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="15">
+      <c r="A72" s="6">
         <v>3</v>
       </c>
-      <c r="B72" s="15">
+      <c r="B72" s="6">
         <v>0.85809999999999997</v>
       </c>
-      <c r="C72" s="15">
+      <c r="C72" s="6">
         <v>12.7072</v>
       </c>
-      <c r="D72" s="14"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="15">
+      <c r="A73" s="6">
         <v>4</v>
       </c>
-      <c r="B73" s="15">
+      <c r="B73" s="6">
         <v>0.86719999999999997</v>
       </c>
-      <c r="C73" s="15">
+      <c r="C73" s="6">
         <v>11.2346</v>
       </c>
-      <c r="D73" s="14"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="15">
+      <c r="A74" s="6">
         <v>5</v>
       </c>
-      <c r="B74" s="15">
+      <c r="B74" s="6">
         <v>0.86299999999999999</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C74" s="6">
         <v>9.9821000000000009</v>
       </c>
-      <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="15">
+      <c r="B75" s="6">
         <f>AVERAGE(B70:B74)</f>
         <v>0.86021999999999998</v>
       </c>
-      <c r="C75" s="15">
+      <c r="C75" s="6">
         <f>AVERAGE(C70:C74)</f>
         <v>10.390499999999999</v>
       </c>
-      <c r="D75" s="14"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="15">
+      <c r="B76" s="6">
         <f>_xlfn.STDEV.S(B70:B74)</f>
         <v>5.8768188673805266E-3</v>
       </c>
-      <c r="C76" s="15">
+      <c r="C76" s="6">
         <f>_xlfn.STDEV.S(C70:C74)</f>
         <v>1.6361521521545561</v>
       </c>
-      <c r="D76" s="14"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
@@ -9603,104 +9631,90 @@
       <c r="C78" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="14"/>
       <c r="E78" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="15">
+      <c r="A79" s="6">
         <v>1</v>
       </c>
-      <c r="B79" s="15">
+      <c r="B79" s="6">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C79" s="15">
+      <c r="C79" s="6">
         <v>11.2805</v>
       </c>
-      <c r="D79" s="14"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="15">
+      <c r="A80" s="6">
         <v>2</v>
       </c>
-      <c r="B80" s="15">
+      <c r="B80" s="6">
         <v>0.43120000000000003</v>
       </c>
-      <c r="C80" s="15">
+      <c r="C80" s="6">
         <v>27.525300000000001</v>
       </c>
-      <c r="D80" s="14"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="15">
+      <c r="A81" s="6">
         <v>3</v>
       </c>
-      <c r="B81" s="15">
+      <c r="B81" s="6">
         <v>0.42699999999999999</v>
       </c>
-      <c r="C81" s="15">
+      <c r="C81" s="6">
         <v>19.981999999999999</v>
       </c>
-      <c r="D81" s="14"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="15">
+      <c r="A82" s="6">
         <v>4</v>
       </c>
-      <c r="B82" s="15">
+      <c r="B82" s="6">
         <v>0.43169999999999997</v>
       </c>
-      <c r="C82" s="15">
+      <c r="C82" s="6">
         <v>22.498699999999999</v>
       </c>
-      <c r="D82" s="14"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="15">
+      <c r="A83" s="6">
         <v>5</v>
       </c>
-      <c r="B83" s="15">
+      <c r="B83" s="6">
         <v>0.43180000000000002</v>
       </c>
-      <c r="C83" s="15">
+      <c r="C83" s="6">
         <v>15.787800000000001</v>
       </c>
-      <c r="D83" s="14"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B84" s="15">
+      <c r="B84" s="6">
         <f>AVERAGE(B79:B83)</f>
         <v>0.49933999999999995</v>
       </c>
-      <c r="C84" s="15">
+      <c r="C84" s="6">
         <f>AVERAGE(C79:C83)</f>
         <v>19.414860000000001</v>
       </c>
-      <c r="D84" s="14"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="16" t="s">
+      <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="15">
+      <c r="B85" s="6">
         <f>_xlfn.STDEV.S(B79:B83)</f>
         <v>0.15411147913117967</v>
       </c>
-      <c r="C85" s="15">
+      <c r="C85" s="6">
         <f>_xlfn.STDEV.S(C79:C83)</f>
         <v>6.2236309894626638</v>
       </c>
-      <c r="D85" s="14"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
@@ -9712,110 +9726,90 @@
       <c r="C87" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D87" s="14"/>
       <c r="E87" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="15">
+      <c r="A88" s="6">
         <v>1</v>
       </c>
-      <c r="B88" s="15">
+      <c r="B88" s="6">
         <v>0.88829999999999998</v>
       </c>
-      <c r="C88" s="15">
+      <c r="C88" s="6">
         <v>9.7341999999999995</v>
       </c>
-      <c r="D88" s="14"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="15">
+      <c r="A89" s="6">
         <v>2</v>
       </c>
-      <c r="B89" s="15">
+      <c r="B89" s="6">
         <v>0.86319999999999997</v>
       </c>
-      <c r="C89" s="15">
+      <c r="C89" s="6">
         <v>13.1211</v>
       </c>
-      <c r="D89" s="14"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="15">
+      <c r="A90" s="6">
         <v>3</v>
       </c>
-      <c r="B90" s="15">
+      <c r="B90" s="6">
         <v>0.86960000000000004</v>
       </c>
-      <c r="C90" s="15">
+      <c r="C90" s="6">
         <v>12.1736</v>
       </c>
-      <c r="D90" s="14"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="15">
+      <c r="A91" s="6">
         <v>4</v>
       </c>
-      <c r="B91" s="15">
+      <c r="B91" s="6">
         <v>0.85389999999999999</v>
       </c>
-      <c r="C91" s="15">
+      <c r="C91" s="6">
         <v>11.2583</v>
       </c>
-      <c r="D91" s="14"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="15">
+      <c r="A92" s="6">
         <v>5</v>
       </c>
-      <c r="B92" s="15">
+      <c r="B92" s="6">
         <v>0.86839999999999995</v>
       </c>
-      <c r="C92" s="15">
+      <c r="C92" s="6">
         <v>9.0557999999999996</v>
       </c>
-      <c r="D92" s="14"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
+      <c r="A93" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B93" s="15">
+      <c r="B93" s="6">
         <f>AVERAGE(B88:B92)</f>
         <v>0.86868000000000001</v>
       </c>
-      <c r="C93" s="15">
+      <c r="C93" s="6">
         <f>AVERAGE(C88:C92)</f>
         <v>11.0686</v>
       </c>
-      <c r="D93" s="14"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+      <c r="A94" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B94" s="15">
+      <c r="B94" s="6">
         <f>_xlfn.STDEV.S(B88:B92)</f>
         <v>1.2593133049404345E-2</v>
       </c>
-      <c r="C94" s="15">
+      <c r="C94" s="6">
         <f>_xlfn.STDEV.S(C88:C92)</f>
         <v>1.6809041123752455</v>
       </c>
-      <c r="D94" s="14"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="14"/>
     </row>
     <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102">
@@ -11372,7 +11366,7 @@
   <dimension ref="A1:R107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11895,13 +11889,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M17">
         <f>_xlfn.T.TEST(N2:N11, 'Standard Training'!B16:B25, 2, 3)</f>
         <v>0.91657178119352722</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -11922,7 +11916,7 @@
         <v>0.86228730050467084</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>0</v>
       </c>
@@ -11940,7 +11934,7 @@
         <v>1.6427687072287007E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -11957,8 +11951,17 @@
         <f>_xlfn.T.TEST('Class-Based Contrastive'!C2:C11, SimCLR!C2:C11, 2, 3)</f>
         <v>1.9872755606033248E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>2</v>
       </c>
@@ -11968,8 +11971,17 @@
       <c r="C21" s="6">
         <v>100.5758</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="3">
+        <v>1</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.30109999999999998</v>
+      </c>
+      <c r="O21" s="4">
+        <v>33.847000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>3</v>
       </c>
@@ -11979,8 +11991,17 @@
       <c r="C22" s="6">
         <v>73.126300000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="5">
+        <v>2</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0.28270000000000001</v>
+      </c>
+      <c r="O22" s="6">
+        <v>29.665299999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>4</v>
       </c>
@@ -11990,8 +12011,17 @@
       <c r="C23" s="6">
         <v>84.174199999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="3">
+        <v>3</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0.3004</v>
+      </c>
+      <c r="O23" s="4">
+        <v>28.931100000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -12003,8 +12033,17 @@
         <f>AVERAGE(C16:C23)</f>
         <v>82.569220000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="5">
+        <v>4</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0.3014</v>
+      </c>
+      <c r="O24" s="6">
+        <v>34.869900000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>6</v>
       </c>
@@ -12016,8 +12055,28 @@
         <f>_xlfn.STDEV.S(C19:C24)</f>
         <v>10.566576153399973</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="3">
+        <v>5</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.2848</v>
+      </c>
+      <c r="O25" s="4">
+        <v>36.154800000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" s="5">
+        <v>6</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0.28360000000000002</v>
+      </c>
+      <c r="O26" s="6">
+        <v>36.520000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
@@ -12030,8 +12089,17 @@
       <c r="E27" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="3">
+        <v>7</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="O27" s="4">
+        <v>40.883299999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>0</v>
       </c>
@@ -12041,8 +12109,17 @@
       <c r="C28" s="6">
         <v>40.696899999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="5">
+        <v>8</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0.28289999999999998</v>
+      </c>
+      <c r="O28" s="6">
+        <v>51.175899999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -12052,8 +12129,17 @@
       <c r="C29" s="6">
         <v>37.058</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="3">
+        <v>9</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="O29" s="4">
+        <v>44.667299999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>2</v>
       </c>
@@ -12063,8 +12149,17 @@
       <c r="C30" s="6">
         <v>36.590899999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="5">
+        <v>10</v>
+      </c>
+      <c r="N30" s="6">
+        <v>0.28079999999999999</v>
+      </c>
+      <c r="O30" s="6">
+        <v>37.615600000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>3</v>
       </c>
@@ -12074,8 +12169,19 @@
       <c r="C31" s="6">
         <v>27.7348</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N31" s="4">
+        <f>AVERAGE(N21:N30)</f>
+        <v>0.28737000000000001</v>
+      </c>
+      <c r="O31" s="4">
+        <f t="shared" ref="O31" si="8">AVERAGE(O21:O30)</f>
+        <v>37.433019999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>4</v>
       </c>
@@ -12084,6 +12190,17 @@
       </c>
       <c r="C32" s="6">
         <v>53.381300000000003</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" s="6">
+        <f>_xlfn.STDEV.S(N21:N30)</f>
+        <v>9.7439496897077319E-3</v>
+      </c>
+      <c r="O32" s="6">
+        <f t="shared" ref="O32" si="9">_xlfn.STDEV.S(O21:O30)</f>
+        <v>6.7301644234165634</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -12111,6 +12228,9 @@
         <f>_xlfn.STDEV.S(C28:C33)</f>
         <v>8.8663949677873646</v>
       </c>
+      <c r="M34" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
@@ -12495,7 +12615,7 @@
         <v>0.84058999999999995</v>
       </c>
       <c r="C65" s="6">
-        <f t="shared" ref="C65" si="8">AVERAGE(C55:C64)</f>
+        <f t="shared" ref="C65" si="10">AVERAGE(C55:C64)</f>
         <v>16.649740000000001</v>
       </c>
     </row>
@@ -12508,7 +12628,7 @@
         <v>1.5752139184532634E-2</v>
       </c>
       <c r="C66" s="10">
-        <f t="shared" ref="C66" si="9">_xlfn.STDEV.S(C55:C64)</f>
+        <f t="shared" ref="C66" si="11">_xlfn.STDEV.S(C55:C64)</f>
         <v>4.8234779709251283</v>
       </c>
     </row>
@@ -12972,8 +13092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34D92F3-DA9B-4EB2-80D8-46C073400D29}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13369,12 +13489,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -13394,8 +13514,17 @@
         <f>_xlfn.T.TEST(B2:B11, SimCLR!B2:B11, 2, 3)</f>
         <v>7.8989740317153723E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>0</v>
       </c>
@@ -13412,8 +13541,17 @@
         <f>_xlfn.T.TEST(C2:C11, SimCLR!C2:C11, 2, 3)</f>
         <v>1.2495868391070274E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.28789999999999999</v>
+      </c>
+      <c r="K19" s="4">
+        <v>34.692100000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -13423,8 +13561,17 @@
       <c r="C20" s="6">
         <v>40.997399999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="5">
+        <v>2</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0.29330000000000001</v>
+      </c>
+      <c r="K20" s="6">
+        <v>40.370899999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>2</v>
       </c>
@@ -13434,8 +13581,17 @@
       <c r="C21" s="6">
         <v>44.982300000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.29020000000000001</v>
+      </c>
+      <c r="K21" s="4">
+        <v>27.4588</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>3</v>
       </c>
@@ -13445,8 +13601,17 @@
       <c r="C22" s="6">
         <v>57.547899999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="5">
+        <v>4</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0.28270000000000001</v>
+      </c>
+      <c r="K22" s="6">
+        <v>46.695900000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>4</v>
       </c>
@@ -13456,8 +13621,17 @@
       <c r="C23" s="6">
         <v>37.638800000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="3">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.29020000000000001</v>
+      </c>
+      <c r="K23" s="4">
+        <v>33.367100000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -13469,8 +13643,17 @@
         <f>AVERAGE(C19:C23)</f>
         <v>47.92266</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="5">
+        <v>6</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0.28249999999999997</v>
+      </c>
+      <c r="K24" s="6">
+        <v>30.898599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>6</v>
       </c>
@@ -13482,8 +13665,28 @@
         <f>_xlfn.STDEV.S(C19:C23)</f>
         <v>9.5625257141092241</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="3">
+        <v>7</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="K25" s="4">
+        <v>20.4285</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I26" s="5">
+        <v>8</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0.28179999999999999</v>
+      </c>
+      <c r="K26" s="6">
+        <v>36.921599999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
@@ -13496,8 +13699,17 @@
       <c r="E27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="3">
+        <v>9</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.29289999999999999</v>
+      </c>
+      <c r="K27" s="4">
+        <v>31.611799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>0</v>
       </c>
@@ -13507,8 +13719,17 @@
       <c r="C28" s="6">
         <v>59.244900000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="5">
+        <v>10</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0.26319999999999999</v>
+      </c>
+      <c r="K28" s="6">
+        <v>33.110799999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -13518,8 +13739,19 @@
       <c r="C29" s="6">
         <v>39.353499999999997</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="4">
+        <f>AVERAGE(J19:J28)</f>
+        <v>0.31028</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" ref="K29" si="6">AVERAGE(K19:K28)</f>
+        <v>33.555610000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>2</v>
       </c>
@@ -13529,8 +13761,19 @@
       <c r="C30" s="6">
         <v>41.850999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="6">
+        <f>_xlfn.STDEV.S(J19:J28)</f>
+        <v>8.0525797108752697E-2</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" ref="K30" si="7">_xlfn.STDEV.S(K19:K28)</f>
+        <v>7.0891191884229592</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>3</v>
       </c>
@@ -13541,7 +13784,7 @@
         <v>53.451999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>4</v>
       </c>
@@ -13550,6 +13793,9 @@
       </c>
       <c r="C32" s="6">
         <v>44.987299999999998</v>
+      </c>
+      <c r="I32" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -14241,7 +14487,7 @@
         <v>0.88240999999999992</v>
       </c>
       <c r="C97" s="6">
-        <f t="shared" ref="C97" si="6">AVERAGE(C87:C96)</f>
+        <f t="shared" ref="C97" si="8">AVERAGE(C87:C96)</f>
         <v>9.4852499999999988</v>
       </c>
     </row>
@@ -14254,7 +14500,7 @@
         <v>2.8672846233171727E-2</v>
       </c>
       <c r="C98" s="10">
-        <f t="shared" ref="C98" si="7">_xlfn.STDEV.S(C87:C96)</f>
+        <f t="shared" ref="C98" si="9">_xlfn.STDEV.S(C87:C96)</f>
         <v>1.8364945456252051</v>
       </c>
     </row>

</xml_diff>